<commit_message>
Added Demonstration Video & Project Report
</commit_message>
<xml_diff>
--- a/JobPosting.xlsx
+++ b/JobPosting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywkxw\Desktop\Wai Kit\Temasek Polytechnic\Y3S2\Core Subjects\Intelligent Automation\Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ywkxw\Desktop\Wai Kit\Temasek Polytechnic\Y3S2\Core Subjects\Intelligent Automation\Project\Applicant Screener\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72ED4F6-976C-4D86-A3ED-620A978B9D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D01925D1-503F-49FC-9C3A-C67BB37DF9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{993D0A36-73CE-4C7D-A2C2-7E30ACA12291}"/>
+    <workbookView xWindow="-28920" yWindow="-2475" windowWidth="29040" windowHeight="15720" xr2:uid="{993D0A36-73CE-4C7D-A2C2-7E30ACA12291}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -452,9 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{323B94A6-4362-4456-9B01-66663E6D9CE8}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>

</xml_diff>